<commit_message>
fix: style changes for test page and added superscript test sample for questions html
</commit_message>
<xml_diff>
--- a/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate-2.xlsx
+++ b/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate-2.xlsx
@@ -311,9 +311,6 @@
     <t>0.732</t>
   </si>
   <si>
-    <t xml:space="preserve"> If both 112 and 33 are factors of the number a * 43 * 62 * 1311, then what is the smallest possible value of a? </t>
-  </si>
-  <si>
     <t xml:space="preserve"> A bag contains 10 balls numbered from 0 to 9. The balls are such that the person picking a ball out of the bag is equally likely to pick anyone of them. A person picked a ball and replaced it in the bag after noting its number. He repeated this process 2 more times. What is the probability that the ball picked first is numbered higher than the ball picked second and the ball picked second is numbered higher than the ball picked third? </t>
   </si>
   <si>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>https://pdwckq.bl3302.livefilestore.com/y3mOOzuZZeORWQrZwBApd1-MK3LwnhsqkGYdYP4crejpMNKmwMxuyPZE3CabrGL0S34W7X8AG0F8pV9EGS8UYSYslxoeNe2r6C09RSwD9mOqfrGnHnmD_GU7e1gKxyK1rqmK1tfDdaJ_jpQDCFewcuKC7W5NgHJ-qOpixnU2JryGHE?width=646&amp;height=243&amp;cropmode=none</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If both 11&lt;sup&gt;2&lt;/sup&gt; and 3&lt;sup&gt;3&lt;/sup&gt; are factors of the number a * 43 * 62 * 1311, then what is the smallest possible value of a? </t>
   </si>
 </sst>
 </file>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +843,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
@@ -882,7 +882,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>17</v>
@@ -921,7 +921,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>18</v>
@@ -960,7 +960,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>17</v>
@@ -999,7 +999,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>17</v>
@@ -1038,7 +1038,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>16</v>
@@ -1077,7 +1077,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>16</v>
@@ -1116,7 +1116,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>18</v>
@@ -1155,7 +1155,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>17</v>
@@ -1194,7 +1194,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>17</v>
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>49</v>
@@ -1238,7 +1238,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>17</v>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>49</v>
@@ -1281,7 +1281,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>17</v>
@@ -1290,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>49</v>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>16</v>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O14" s="1"/>
     </row>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>16</v>
@@ -1378,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O15" s="1"/>
     </row>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>16</v>
@@ -1421,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -1453,7 +1453,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>16</v>
@@ -1492,7 +1492,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>17</v>
@@ -1531,7 +1531,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>17</v>
@@ -1570,7 +1570,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>16</v>
@@ -1609,7 +1609,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>17</v>
@@ -1646,7 +1646,7 @@
         <v>79</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>17</v>
@@ -1681,7 +1681,7 @@
         <v>84</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>16</v>
@@ -1716,7 +1716,7 @@
         <v>89</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>17</v>
@@ -1751,7 +1751,7 @@
         <v>94</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>16</v>
@@ -1765,7 +1765,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -1786,7 +1786,7 @@
         <v>33</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>17</v>
@@ -1800,7 +1800,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -1809,19 +1809,19 @@
         <v>172</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="K27" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>17</v>
@@ -1835,7 +1835,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -1856,7 +1856,7 @@
         <v>12</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>16</v>
@@ -1870,7 +1870,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1891,7 +1891,7 @@
         <v>3666.66</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>17</v>
@@ -1905,7 +1905,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1914,19 +1914,19 @@
         <v>172</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="K30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>16</v>
@@ -1940,7 +1940,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1961,7 +1961,7 @@
         <v>740</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fix: style fixes and blur in flipclock fixed
</commit_message>
<xml_diff>
--- a/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate-2.xlsx
+++ b/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate-2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="117">
   <si>
     <t>Id</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t xml:space="preserve"> If both 11&lt;sup&gt;2&lt;/sup&gt; and 3&lt;sup&gt;3&lt;/sup&gt; are factors of the number a * 43 * 62 * 1311, then what is the smallest possible value of a? </t>
+  </si>
+  <si>
+    <t>IsRadio</t>
   </si>
 </sst>
 </file>
@@ -748,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +771,7 @@
     <col min="15" max="15" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,8 +817,11 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -853,8 +859,11 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -892,8 +901,11 @@
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -932,7 +944,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -971,7 +983,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1010,7 +1022,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1049,7 +1061,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1088,7 +1100,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1127,7 +1139,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1166,7 +1178,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1209,7 +1221,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1253,7 +1265,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1296,7 +1308,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1339,7 +1351,7 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1382,7 +1394,7 @@
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>